<commit_message>
letting finished without formatting end date
</commit_message>
<xml_diff>
--- a/gnb_di_test.xlsx
+++ b/gnb_di_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\phpDatamigration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DBC63B-D5E2-40D3-853E-B9107AD4D33B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00141FD1-55D6-4CCB-B4B9-FF6A2E7AFAFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="7452" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
   <si>
     <t>Property Category</t>
   </si>
@@ -160,12 +160,6 @@
     <t>Property Price</t>
   </si>
   <si>
-    <t>+91-9090900909</t>
-  </si>
-  <si>
-    <t>+444567 9087</t>
-  </si>
-  <si>
     <t>mmdg@mc.com</t>
   </si>
   <si>
@@ -323,12 +317,48 @@
   </si>
   <si>
     <t>Dr Ambedkar Nagar</t>
+  </si>
+  <si>
+    <t>444567 9087</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>9090900909</t>
+  </si>
+  <si>
+    <t>8909800012</t>
+  </si>
+  <si>
+    <t>1230985674</t>
+  </si>
+  <si>
+    <t>2018-11-02</t>
+  </si>
+  <si>
+    <t>2019-03-27</t>
+  </si>
+  <si>
+    <t>2018-11-01</t>
+  </si>
+  <si>
+    <t>2019-08-21</t>
+  </si>
+  <si>
+    <t>2019-05-01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -343,10 +373,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
       <color rgb="FF111827"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -373,10 +403,9 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -389,11 +418,21 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -762,9 +801,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -773,16 +812,19 @@
     <col min="2" max="2" width="10.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17.109375" style="6" customWidth="1"/>
+    <col min="9" max="10" width="17.109375" style="5" customWidth="1"/>
     <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.88671875" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" style="11" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" customWidth="1"/>
     <col min="15" max="15" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="25.6640625" style="4" customWidth="1"/>
-    <col min="18" max="19" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="25.6640625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7.5546875" customWidth="1"/>
     <col min="21" max="21" width="19" customWidth="1"/>
     <col min="22" max="22" width="32.88671875" bestFit="1" customWidth="1"/>
@@ -790,10 +832,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="49.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C1" t="s">
@@ -805,66 +847,66 @@
       <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>97</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>79</v>
+        <v>95</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="O1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>49</v>
+      <c r="T1" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="U1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" t="s">
         <v>54</v>
-      </c>
-      <c r="V1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="3">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2">
         <v>258</v>
       </c>
       <c r="C2" t="s">
@@ -876,67 +918,66 @@
       <c r="E2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>88</v>
+      <c r="F2" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>5450</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>27250</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>27250</v>
       </c>
       <c r="L2" s="1">
         <v>0.08</v>
       </c>
-      <c r="M2" s="11">
-        <f>K2 * (L2 / 100)</f>
+      <c r="M2" s="15">
         <v>21.8</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O2" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>1234567890</v>
-      </c>
-      <c r="R2" s="2">
-        <v>43406</v>
-      </c>
-      <c r="S2" s="2">
+      <c r="P2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>99</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="S2" s="3">
         <v>43771</v>
       </c>
       <c r="T2">
         <v>1</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="V2" t="s">
-        <v>70</v>
-      </c>
-      <c r="W2">
-        <v>1234567890</v>
+        <v>68</v>
+      </c>
+      <c r="W2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="2">
         <v>274</v>
       </c>
       <c r="C3" t="s">
@@ -948,8 +989,8 @@
       <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>89</v>
+      <c r="F3" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>36</v>
@@ -957,47 +998,48 @@
       <c r="H3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>8250000</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>0</v>
       </c>
       <c r="L3" s="1">
         <v>0.08</v>
       </c>
-      <c r="M3" s="11">
-        <f t="shared" ref="M3:M9" si="0">K3 * (L3 / 100)</f>
+      <c r="M3" s="15">
         <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O3" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="4">
-        <v>1234567890</v>
-      </c>
-      <c r="S3"/>
+      <c r="Q3" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="T3">
         <v>2</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="U3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="W3">
-        <v>1234567890</v>
+      <c r="W3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="3">
+        <v>61</v>
+      </c>
+      <c r="B4" s="2">
         <v>53</v>
       </c>
       <c r="C4" t="s">
@@ -1009,8 +1051,8 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>90</v>
+      <c r="F4" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="G4" t="s">
         <v>36</v>
@@ -1018,58 +1060,57 @@
       <c r="H4" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>3425000</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>34250000</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>34250000</v>
       </c>
       <c r="L4" s="1">
         <v>0.1</v>
       </c>
-      <c r="M4" s="11">
-        <f t="shared" si="0"/>
+      <c r="M4" s="15">
         <v>34250</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="O4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>1234567890</v>
-      </c>
-      <c r="R4" s="2">
-        <v>43551</v>
-      </c>
-      <c r="S4" t="s">
-        <v>51</v>
+      <c r="P4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="T4">
         <v>4</v>
       </c>
-      <c r="U4" s="5" t="s">
+      <c r="U4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="V4" t="s">
-        <v>72</v>
-      </c>
-      <c r="W4">
-        <v>1234567890</v>
+        <v>70</v>
+      </c>
+      <c r="W4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="3">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2">
         <v>6</v>
       </c>
       <c r="C5" t="s">
@@ -1081,8 +1122,8 @@
       <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>91</v>
+      <c r="F5" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="G5" t="s">
         <v>36</v>
@@ -1090,53 +1131,54 @@
       <c r="H5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>5580000</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>0</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>0</v>
       </c>
       <c r="L5" s="1">
         <v>0.1</v>
       </c>
-      <c r="M5" s="11">
-        <f t="shared" si="0"/>
+      <c r="M5" s="15">
         <v>0</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O5" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>987654321</v>
-      </c>
-      <c r="S5"/>
+      <c r="P5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="T5">
         <v>5</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="V5" t="s">
-        <v>74</v>
-      </c>
-      <c r="W5">
-        <v>987654321</v>
+        <v>72</v>
+      </c>
+      <c r="W5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C6" t="s">
@@ -1148,64 +1190,63 @@
       <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>88</v>
+      <c r="F6" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>25000</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>0</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>0</v>
       </c>
       <c r="L6" s="1">
         <v>0.1</v>
       </c>
-      <c r="M6" s="11">
-        <f t="shared" si="0"/>
+      <c r="M6" s="15">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O6" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q6" s="9" t="s">
+      <c r="P6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="2">
-        <v>43405</v>
-      </c>
-      <c r="S6" t="s">
-        <v>52</v>
+      <c r="Q6" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="T6">
         <v>6</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="U6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="W6" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
@@ -1217,67 +1258,66 @@
       <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>92</v>
+      <c r="F7" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H7" t="s">
         <v>35</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>18000</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>0</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>0.08</v>
       </c>
-      <c r="M7" s="11">
-        <f t="shared" si="0"/>
+      <c r="M7" s="15">
         <v>0</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O7" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>8909800012</v>
-      </c>
-      <c r="R7" s="2">
-        <v>43698</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="P7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>37</v>
       </c>
       <c r="T7">
         <v>7</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="U7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="V7" t="s">
-        <v>76</v>
-      </c>
-      <c r="W7">
-        <v>8909800012</v>
+        <v>74</v>
+      </c>
+      <c r="W7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="66" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="3">
+        <v>65</v>
+      </c>
+      <c r="B8" s="2">
         <v>75</v>
       </c>
       <c r="C8" t="s">
@@ -1289,71 +1329,70 @@
       <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" t="s">
         <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>95</v>
       </c>
       <c r="H8" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>12500</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>75000</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>75000</v>
       </c>
       <c r="L8" s="1">
         <v>0.1</v>
       </c>
-      <c r="M8" s="11">
-        <f t="shared" si="0"/>
+      <c r="M8" s="15">
         <v>75</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O8" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>1230985674</v>
-      </c>
-      <c r="R8" s="2">
-        <v>43586</v>
-      </c>
-      <c r="S8" t="s">
-        <v>53</v>
+      <c r="P8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="T8">
         <v>8</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="U8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="V8" t="s">
-        <v>78</v>
-      </c>
-      <c r="W8">
-        <v>1230985674</v>
+        <v>76</v>
+      </c>
+      <c r="W8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="3">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2">
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -1361,8 +1400,8 @@
       <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>94</v>
+      <c r="F9" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="G9" t="s">
         <v>36</v>
@@ -1370,55 +1409,53 @@
       <c r="H9" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>4250000</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>12750000</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>12750000</v>
       </c>
       <c r="L9" s="1">
         <v>0.1</v>
       </c>
-      <c r="M9" s="11">
-        <f t="shared" si="0"/>
+      <c r="M9" s="15">
         <v>12750</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O9" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q9" s="9" t="s">
+      <c r="P9" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="S9" s="2" t="s">
-        <v>96</v>
+      <c r="Q9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="T9">
         <v>9</v>
       </c>
-      <c r="U9" s="5" t="s">
+      <c r="U9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="W9" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <hyperlinks>
-    <hyperlink ref="P6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="P9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>